<commit_message>
Made changes to the AI Energy mappings
</commit_message>
<xml_diff>
--- a/data/AI Energy Consumption Dataset.xlsx
+++ b/data/AI Energy Consumption Dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Works\SustAIn\SustAIn-Backend\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Works\SustAIn\SustAIn-Backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED2EC21-1F83-4036-B2A6-EEAA87E452AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A791E46C-2BE9-4928-85AC-EA09F78158FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{38D89E16-535F-4CA5-8C40-947D5B651D0F}"/>
   </bookViews>
@@ -408,7 +408,7 @@
     <t>Formula Used :</t>
   </si>
   <si>
-    <t>b - efficiency gains (0.7)</t>
+    <t>b - efficiency gains</t>
   </si>
 </sst>
 </file>
@@ -474,8 +474,8 @@
       <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1496307" cy="345479"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -517,6 +517,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -692,7 +693,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1058,7 +1059,7 @@
   <dimension ref="A1:M110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1136,28 +1137,28 @@
         <v>14</v>
       </c>
       <c r="H2">
-        <f>(POWER((1750/G2),0.7)*E2)</f>
-        <v>0.84399821504019501</v>
+        <f>(POWER((1750/G2),J20)*E2)</f>
+        <v>2.2167847786702231</v>
       </c>
       <c r="I2">
-        <f>(POWER((170/G2),0.7)*E2)</f>
-        <v>0.16501717160274817</v>
+        <f>(POWER((170/G2),J20)*E2)</f>
+        <v>0.27189005099502084</v>
       </c>
       <c r="J2">
-        <f>(POWER((1500/G2),0.7)*E2)</f>
-        <v>0.75766770364704183</v>
+        <f>(POWER((1500/G2),J20)*E2)</f>
+        <v>1.929618348259025</v>
       </c>
       <c r="K2">
-        <f>(POWER((200/G2),0.7)*E2)</f>
-        <v>0.18489956568163157</v>
+        <f>(POWER((200/G2),J20)*E2)</f>
+        <v>0.31471415954324367</v>
       </c>
       <c r="L2">
-        <f>(POWER((70/G2),0.7)*E2)</f>
-        <v>8.8671391146808859E-2</v>
+        <f>(POWER((70/G2),J20)*E2)</f>
+        <v>0.12234254848828158</v>
       </c>
       <c r="M2">
-        <f>(POWER((13/G2),0.7)*E2)</f>
-        <v>2.7288222070016546E-2</v>
+        <f>(POWER((13/G2),J20)*E2)</f>
+        <v>2.6886749689739291E-2</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1196,28 +1197,28 @@
         <v>11</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H3:H12" si="0">(POWER((1750/G4),0.7)*E4)</f>
-        <v>0.9660389790305266</v>
+        <f>(POWER((1750/G4),J20)*E4)</f>
+        <v>2.6627091027701124</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I3:I12" si="1">(POWER((170/G4),0.7)*E4)</f>
-        <v>0.18887838521084099</v>
+        <f>(POWER((170/G4),J20)*E4)</f>
+        <v>0.32658295054306319</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J3:J10" si="2">(POWER((1500/G4),0.7)*E4)</f>
-        <v>0.86722521663240049</v>
+        <f>(POWER((1500/G4),J20)*E4)</f>
+        <v>2.317776804595197</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K3:K10" si="3">(POWER((200/G4),0.7)*E4)</f>
-        <v>0.21163574101369942</v>
+        <f>(POWER((200/G4),J20)*E4)</f>
+        <v>0.37802147752436543</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L3:L10" si="4">(POWER((70/G4),0.7)*E4)</f>
-        <v>0.1014931295424603</v>
+        <f>(POWER((70/G4),J20)*E4)</f>
+        <v>0.14695274915738815</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M3:M10" si="5">(POWER((13/G4),0.7)*E4)</f>
-        <v>3.1234054430816109E-2</v>
+        <f>(POWER((13/G4),J20)*E4)</f>
+        <v>3.2295238505614346E-2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1256,28 +1257,28 @@
         <v>11</v>
       </c>
       <c r="H6">
-        <f>(POWER((1750/G6),0.7)*E6)</f>
-        <v>1.210097827691099</v>
+        <f>(POWER((1750/G6),J20)*E6)</f>
+        <v>3.3354125154132208</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
-        <v>0.23659637820289112</v>
+        <f>(POWER((170/G6),J20)*E6)</f>
+        <v>0.40909044830645724</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
-        <v>1.086319883095161</v>
+        <f>(POWER((1500/G6),J20)*E6)</f>
+        <v>2.9033369638233153</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
-        <v>0.26510312318813894</v>
+        <f>(POWER((200/G6),J20)*E6)</f>
+        <v>0.47352433877138522</v>
       </c>
       <c r="L6">
-        <f t="shared" si="4"/>
-        <v>0.1271342236191709</v>
+        <f>(POWER((70/G6),J20)*E6)</f>
+        <v>0.18407870322898334</v>
       </c>
       <c r="M6">
-        <f t="shared" si="5"/>
-        <v>3.912498588270915E-2</v>
+        <f>(POWER((13/G6),J20)*E6)</f>
+        <v>4.0454266141133545E-2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1315,28 +1316,28 @@
         <v>11</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>0.88606454988872074</v>
+        <f>(POWER((1750/G8),J20)*E8)</f>
+        <v>2.4422742703387796</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
-        <v>0.17324191363738309</v>
+        <f>(POWER((170/G8),J20)*E8)</f>
+        <v>0.29954647934048373</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
-        <v>0.79543117607809743</v>
+        <f>(POWER((1500/G8),J20)*E8)</f>
+        <v>2.1258975110581582</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
-        <v>0.1941152807207211</v>
+        <f>(POWER((200/G8),J20)*E8)</f>
+        <v>0.34672662035546253</v>
       </c>
       <c r="L8">
-        <f t="shared" si="4"/>
-        <v>9.3090927071169421E-2</v>
+        <f>(POWER((70/G8),J20)*E8)</f>
+        <v>0.13478713008839846</v>
       </c>
       <c r="M8">
-        <f t="shared" si="5"/>
-        <v>2.8648314386045433E-2</v>
+        <f>(POWER((13/G8),J20)*E8)</f>
+        <v>2.9621647357069854E-2</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1375,28 +1376,28 @@
         <v>6.6</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>81.517115597209767</v>
+        <f>(POWER((1750/G10),J20)*E10)</f>
+        <v>248.85571958400158</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
-        <v>15.938095144460929</v>
+        <f>(POWER((170/G10),J20)*E10)</f>
+        <v>30.522310933894399</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
-        <v>73.178929388525944</v>
+        <f>(POWER((1500/G10),J20)*E10)</f>
+        <v>216.61848601583529</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
-        <v>17.858425528572507</v>
+        <f>(POWER((200/G10),J20)*E10)</f>
+        <v>35.329734934118825</v>
       </c>
       <c r="L10">
-        <f t="shared" si="4"/>
-        <v>8.5642788260346983</v>
+        <f>(POWER((70/G10),J20)*E10)</f>
+        <v>13.73414470937286</v>
       </c>
       <c r="M10">
-        <f t="shared" si="5"/>
-        <v>2.6356183144509746</v>
+        <f>(POWER((13/G10),J20)*E10)</f>
+        <v>3.01829997467263</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1435,12 +1436,12 @@
         <v>9</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
-        <v>0.10567821297431479</v>
+        <f>(POWER((1750/G12),J20)*E12)</f>
+        <v>0.30321073178348501</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
-        <v>2.0662033988097666E-2</v>
+        <f>(POWER((170/G12),J20)*E12)</f>
+        <v>3.7188987456104071E-2</v>
       </c>
       <c r="J12" t="s">
         <v>121</v>
@@ -1485,27 +1486,27 @@
       </c>
       <c r="H14">
         <f>(2.5*H2)</f>
-        <v>2.1099955376004873</v>
+        <v>5.5419619466755581</v>
       </c>
       <c r="I14">
-        <f t="shared" ref="I14:M14" si="6">(2.5*I2)</f>
-        <v>0.41254292900687045</v>
+        <f t="shared" ref="I14:M14" si="0">(2.5*I2)</f>
+        <v>0.67972512748755209</v>
       </c>
       <c r="J14">
-        <f t="shared" si="6"/>
-        <v>1.8941692591176045</v>
+        <f t="shared" si="0"/>
+        <v>4.8240458706475629</v>
       </c>
       <c r="K14">
-        <f t="shared" si="6"/>
-        <v>0.46224891420407893</v>
+        <f t="shared" si="0"/>
+        <v>0.78678539885810916</v>
       </c>
       <c r="L14">
-        <f t="shared" si="6"/>
-        <v>0.22167847786702216</v>
+        <f t="shared" si="0"/>
+        <v>0.30585637122070397</v>
       </c>
       <c r="M14">
-        <f t="shared" si="6"/>
-        <v>6.8220555175041359E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.721687422434823E-2</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1530,7 +1531,7 @@
         <v>5.5938079999999996E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>8.059587E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1555,7 +1556,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1566,7 +1567,7 @@
         <v>1.9130424E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1579,8 +1580,11 @@
       <c r="I20" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1591,7 +1595,7 @@
         <v>1.5875393000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -1602,7 +1606,7 @@
         <v>1.7333139000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1613,7 +1617,7 @@
         <v>1.6441257000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -1624,7 +1628,7 @@
         <v>1.7376262999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1635,7 +1639,7 @@
         <v>2.6102442E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1646,7 +1650,7 @@
         <v>7.7082339999999996E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1657,7 +1661,7 @@
         <v>7.6446229999999997E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1668,7 +1672,7 @@
         <v>7.2795170000000001E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1679,7 +1683,7 @@
         <v>8.0952119999999992E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1690,7 +1694,7 @@
         <v>8.6798110000000008E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1701,7 +1705,7 @@
         <v>1.8899583000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>35</v>
       </c>

</xml_diff>